<commit_message>
Data driven colors for bars (legend implementation)
</commit_message>
<xml_diff>
--- a/documents/Published/GanttChart/GanttChartByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/GanttChart/GanttChartByMAQSoftwareChecklist.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PowerBI\PowerBI-visuals\documents\Published\GanttChart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\documents\Published\GanttChart\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86844A70-3D25-4F24-9412-5045992FFB9E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215" xr2:uid="{15650058-D9E1-4E2D-A421-D272244BB495}"/>
   </bookViews>
@@ -973,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD304B0-4792-43AB-9D20-CD62C2AB01B6}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
1. Tooltip date format used from modeling 2. Tooltip bug fixes 3. Added limit to the maximum number of columns in tooltip bag to 4
</commit_message>
<xml_diff>
--- a/documents/Published/GanttChart/GanttChartByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/GanttChart/GanttChartByMAQSoftwareChecklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\documents\Published\GanttChart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SnehalS\Source\Repos\PowerBI-visuals\documents\Published\GanttChart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86844A70-3D25-4F24-9412-5045992FFB9E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B5D4C0-D995-4E85-A7F5-3EB3ACBD9F67}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215" xr2:uid="{15650058-D9E1-4E2D-A421-D272244BB495}"/>
   </bookViews>
@@ -974,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD304B0-4792-43AB-9D20-CD62C2AB01B6}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Final build after API upgrade
</commit_message>
<xml_diff>
--- a/documents/Published/GanttChart/GanttChartByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/GanttChart/GanttChartByMAQSoftwareChecklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SnehalS\Source\Repos\PowerBI-visuals\documents\Published\GanttChart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualWork\documents\Published\GanttChart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B5D4C0-D995-4E85-A7F5-3EB3ACBD9F67}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F8C838-22C5-4479-9DB2-45032DE49A69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215" xr2:uid="{15650058-D9E1-4E2D-A421-D272244BB495}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="117">
   <si>
     <r>
       <t>#</t>
@@ -480,6 +480,57 @@
   </si>
   <si>
     <t>Format pane must show fill color option for 4 bars and the bar fill color must change to red for the corresponding bar</t>
+  </si>
+  <si>
+    <t>Legend for Category field</t>
+  </si>
+  <si>
+    <t>Display legend for one of the Category field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Drag 'ProjectNane' in 'Legend' field.
+2.  Go to 'Formatting pane'
+3. Go to 'Bar Formatting'
+4. Update 'Color' for all bars
+ </t>
+  </si>
+  <si>
+    <t>Enable Hierarchy layout</t>
+  </si>
+  <si>
+    <t>Hierarchy is enabled for Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Go to 'Formatting pane'
+2.  Go to 'Column labels'
+3. Enable toggle for 'Hierarchial layout'
+ </t>
+  </si>
+  <si>
+    <t>1.Hierarchial layout is enabled for Categories</t>
+  </si>
+  <si>
+    <t>1. Legends for 'ProjectName' will appear
+4. 'Color' will be updated for the legends</t>
+  </si>
+  <si>
+    <t>Bookmarks</t>
+  </si>
+  <si>
+    <t>Check whether bookmarks feature works
+(Note: Won’t work when Hierarchy layout is ON)</t>
+  </si>
+  <si>
+    <t>1. Go to View and turn on Bookmarks Pane
+2. In the visual, perform selections
+3. In the boomarks pane, add a new bookmark such that selections are retained
+4. Now change selections &amp; click on the saved bookmark</t>
+  </si>
+  <si>
+    <t>1. Bookmarks Pane will be visible on the left
+2. Visual will update according to selections
+3. In the boomarks pane, a new entry of the bookmark will come
+4. The selection state saved in bookmark will be restored in the visual</t>
   </si>
 </sst>
 </file>
@@ -972,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD304B0-4792-43AB-9D20-CD62C2AB01B6}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1476,7 +1527,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>14</v>
       </c>
@@ -1502,6 +1553,69 @@
         <v>91</v>
       </c>
       <c r="I19" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>15</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>16</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F22" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" t="s">
+        <v>91</v>
+      </c>
+      <c r="H22" t="s">
+        <v>91</v>
+      </c>
+      <c r="I22" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1809,5 +1923,6 @@
     <mergeCell ref="C21:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bug fixes and API upgrade
</commit_message>
<xml_diff>
--- a/documents/Published/GanttChart/GanttChartByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/GanttChart/GanttChartByMAQSoftwareChecklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualWork\documents\Published\GanttChart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NewGit\documents\Published\GanttChart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F8C838-22C5-4479-9DB2-45032DE49A69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5480135F-4EA6-4075-AAF4-59EDDB3B5161}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215" xr2:uid="{15650058-D9E1-4E2D-A421-D272244BB495}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{15650058-D9E1-4E2D-A421-D272244BB495}"/>
   </bookViews>
   <sheets>
     <sheet name="BVT" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="133">
   <si>
     <r>
       <t>#</t>
@@ -315,15 +315,6 @@
   </si>
   <si>
     <t>1. Go to formatting pane
-2. Go to 'Data labels' option
-3. Switch the toggle on
-4. Update 'Position' to 'Right'
-5. Update 'Color' to 'red'
-6. Update 'Text size' to '30'
-7. Update 'Font family' to 'Arial Black'</t>
-  </si>
-  <si>
-    <t>1. Go to formatting pane
 2. Go to 'Gantt date type' option
 3. Update 'Type' to 'Month'
 4. Update 'Show today indicator' to 'On'</t>
@@ -394,13 +385,6 @@
 3. 'Font family' will be set to 'Arial Black'
 4. Category labels section should be collapsed
 5. Category labels will be displayed in a hierarchical manner</t>
-  </si>
-  <si>
-    <t>1. Data labels will be displayed in chart
-2. 'Position' will be set to 'Right'
-3. 'Color' will be set to 'red'
-4. 'Text size' will be set to 30
-5. 'Font family' will be set to 'Arial Black'</t>
   </si>
   <si>
     <t>Data labels settings</t>
@@ -488,49 +472,121 @@
     <t>Display legend for one of the Category field</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Drag 'ProjectNane' in 'Legend' field.
+    <t>Enable Hierarchy layout</t>
+  </si>
+  <si>
+    <t>Hierarchy is enabled for Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Go to 'Formatting pane'
+2.  Go to 'Column labels'
+3. Enable toggle for 'Hierarchial layout'
+ </t>
+  </si>
+  <si>
+    <t>1.Hierarchial layout is enabled for Categories</t>
+  </si>
+  <si>
+    <t>1. Legends for 'ProjectName' will appear
+4. 'Color' will be updated for the legends</t>
+  </si>
+  <si>
+    <t>Bookmarks</t>
+  </si>
+  <si>
+    <t>Check whether bookmarks feature works
+(Note: Won’t work when Hierarchy layout is ON)</t>
+  </si>
+  <si>
+    <t>1. Go to View and turn on Bookmarks Pane
+2. In the visual, perform selections
+3. In the boomarks pane, add a new bookmark such that selections are retained
+4. Now change selections &amp; click on the saved bookmark</t>
+  </si>
+  <si>
+    <t>1. Bookmarks Pane will be visible on the left
+2. Visual will update according to selections
+3. In the boomarks pane, a new entry of the bookmark will come
+4. The selection state saved in bookmark will be restored in the visual</t>
+  </si>
+  <si>
+    <t>KPI Legend</t>
+  </si>
+  <si>
+    <t>On/Off the KPI Legend</t>
+  </si>
+  <si>
+    <t>1. Go to 'Formatting pane'
+2. On/off the KPI Legend toggle</t>
+  </si>
+  <si>
+    <t>The KPI legend will be shown based on selection</t>
+  </si>
+  <si>
+    <t>In the hierarchy view, Decrease the display ratio</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Display ratio' option
+3. Update 'Ratio' to '15%'</t>
+  </si>
+  <si>
+    <t>1. 'Ratio' will be set to '15%'
+2. Ellipsis will be shown for the category data labels</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Data labels' option
+3. Switch the toggle on
+4. Update 'Position' to 'Left'
+5. Update 'Color' to 'red'
+6. Update 'Text size' to '30'
+7. Update 'Font family' to 'Arial Black'</t>
+  </si>
+  <si>
+    <t>1. Data labels will be displayed in chart
+2. 'Position' will be set to 'Left'
+3. 'Color' will be set to 'red'
+4. 'Text size' will be set to 30
+5. 'Font family' will be set to 'Arial Black'</t>
+  </si>
+  <si>
+    <t>Update 'Position' to 'Center'</t>
+  </si>
+  <si>
+    <t>Update Position of Data labels</t>
+  </si>
+  <si>
+    <t>Position' will be set to 'Left'</t>
+  </si>
+  <si>
+    <t>Display '(Blank)' in tooltip if null data is passed</t>
+  </si>
+  <si>
+    <t>Drag 'Riskstatus' in 'Tooltip' field</t>
+  </si>
+  <si>
+    <t>A tooltip on hover of each bar with Riskstatus should be displayed.
+If Risk Status is null in any case, then Blank should be displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Drag 'ProjectName' in 'Legend' field.
 2.  Go to 'Formatting pane'
 3. Go to 'Bar Formatting'
 4. Update 'Color' for all bars
  </t>
   </si>
   <si>
-    <t>Enable Hierarchy layout</t>
-  </si>
-  <si>
-    <t>Hierarchy is enabled for Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Go to 'Formatting pane'
-2.  Go to 'Column labels'
-3. Enable toggle for 'Hierarchial layout'
- </t>
-  </si>
-  <si>
-    <t>1.Hierarchial layout is enabled for Categories</t>
-  </si>
-  <si>
-    <t>1. Legends for 'ProjectName' will appear
-4. 'Color' will be updated for the legends</t>
-  </si>
-  <si>
-    <t>Bookmarks</t>
-  </si>
-  <si>
-    <t>Check whether bookmarks feature works
-(Note: Won’t work when Hierarchy layout is ON)</t>
-  </si>
-  <si>
-    <t>1. Go to View and turn on Bookmarks Pane
-2. In the visual, perform selections
-3. In the boomarks pane, add a new bookmark such that selections are retained
-4. Now change selections &amp; click on the saved bookmark</t>
-  </si>
-  <si>
-    <t>1. Bookmarks Pane will be visible on the left
-2. Visual will update according to selections
-3. In the boomarks pane, a new entry of the bookmark will come
-4. The selection state saved in bookmark will be restored in the visual</t>
+    <t>Display tooltip on hover</t>
+  </si>
+  <si>
+    <t>A tooltip on hover of each bar with KPI Status should be displayed.</t>
+  </si>
+  <si>
+    <t>1. Drag 'Region'  in 'Category' field, keep 'Legend' data field empty
+2. Drag 'MilestonePhaseStart' in 'Start' field
+3. Drag 'MilestonePhaseFinish' in 'End' field
+4. Drag 'KPI Status'(numeric) column in 'Tooltip' field</t>
   </si>
 </sst>
 </file>
@@ -682,14 +738,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1023,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD304B0-4792-43AB-9D20-CD62C2AB01B6}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,12 +1093,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F1" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="F1" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -1063,16 +1117,16 @@
         <v>43</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G2" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H2" s="11" t="s">
-        <v>92</v>
-      </c>
       <c r="I2" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1092,16 +1146,16 @@
         <v>32</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1109,7 +1163,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>37</v>
@@ -1121,16 +1175,16 @@
         <v>35</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1150,16 +1204,16 @@
         <v>39</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1179,451 +1233,606 @@
         <v>48</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
         <v>5</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B8" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="D8" s="10" t="s">
+      <c r="D9" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="F9" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
         <v>6</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B10" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C10" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
-        <v>7</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>60</v>
-      </c>
       <c r="F10" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
+        <v>7</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
         <v>8</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B12" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C12" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="E11" s="10" t="s">
+      <c r="F12" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>9</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
-        <v>9</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10" t="s">
+      <c r="F13" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
-        <v>10</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>66</v>
-      </c>
       <c r="D14" s="10" t="s">
-        <v>68</v>
+        <v>121</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>69</v>
+        <v>122</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
-        <v>11</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>98</v>
-      </c>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="10" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>70</v>
+        <v>123</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>125</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
+        <v>11</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>12</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
         <v>13</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B19" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C19" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="E19" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="F19" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="F17" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10" t="s">
+      <c r="D20" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="10" t="s">
+      <c r="E20" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>14</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
-        <v>14</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="10" t="s">
+      <c r="E21" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="H19" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I19" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
+      <c r="F21" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
         <v>15</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B23" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>16</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C24" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D24" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E24" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>17</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>18</v>
+      </c>
+      <c r="B26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" s="10" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
-        <v>16</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>15</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="E26" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="F22" t="s">
-        <v>91</v>
-      </c>
-      <c r="G22" t="s">
-        <v>91</v>
-      </c>
-      <c r="H22" t="s">
-        <v>91</v>
-      </c>
-      <c r="I22" t="s">
-        <v>91</v>
+      <c r="F26" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" t="s">
+        <v>89</v>
+      </c>
+      <c r="H26" t="s">
+        <v>89</v>
+      </c>
+      <c r="I26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="138" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>19</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E27" t="s">
+        <v>131</v>
+      </c>
+      <c r="F27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" t="s">
+        <v>89</v>
+      </c>
+      <c r="H27" t="s">
+        <v>89</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="1">
     <mergeCell ref="F1:I1"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>